<commit_message>
Se realizaron cambios en el JSon RyT para añadir iniciativas, asi mismo con en susu componentes para leer este dato
</commit_message>
<xml_diff>
--- a/COMISIÓN DE CULTURA - INTEGRANTES.xlsx
+++ b/COMISIÓN DE CULTURA - INTEGRANTES.xlsx
@@ -5,21 +5,21 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\develop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\develop\ComFichas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FD91C6-6D7F-4266-B7A8-EDA3E1AB1C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3DC0D8-6D51-4EA9-87BE-DA6BCD7E8294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8E893EC4-BED4-4412-9102-0ADB4B7052B2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8E893EC4-BED4-4412-9102-0ADB4B7052B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Cultura Completo" sheetId="1" r:id="rId1"/>
-    <sheet name="Cultura Ficha" sheetId="2" r:id="rId2"/>
-    <sheet name="RyT Completo" sheetId="3" r:id="rId3"/>
+    <sheet name="RyT Completo" sheetId="3" r:id="rId2"/>
+    <sheet name="Cultura Ficha" sheetId="2" r:id="rId3"/>
     <sheet name="RyT Ficha" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Cultura Ficha'!$A$1:$E$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Cultura Ficha'!$A$1:$E$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
@@ -444,7 +444,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="295">
   <si>
     <t xml:space="preserve">ESCOLARIDAD </t>
   </si>
@@ -1323,6 +1323,20 @@
   </si>
   <si>
     <t>CLAUDIA GARCÍA HERNÁNDEZ</t>
+  </si>
+  <si>
+    <t>INICIATIVAS</t>
+  </si>
+  <si>
+    <t>Proyecto de decreto que reforma y adiciona diversas disposiciones de la Ley General de Salud.
+Proyecto de decreto que reforma diversas disposiciones de la Ley General de Salud.
+Proyecto de decreto que reforma el segundo párrafo del artículo 60 y el tercer párrafo del artículo 315; y se deroga el artículo 199 Bis, Capítulo II del Título Séptimo del Libro Segundo, todos del Código Penal Federal, en materia de peligro de contagio.
+Subsecretaria de Servicios de Salud del gobierno de Hidalgo.
+Subsecretaria de Desarrollo Social y Humano del gobierno de Hidalgo.
+Secretaria de Desarrollo Humano y Social del gobierno de Pachuca, Hidalgo.
+Directora del Instituto Municipal de las Mujeres en Pachuca, Hidalgo.
+Coordinadora de la Región Centro del Fondo de Apoyo para las Mujeres del Inmujeres.
+Directora del Refugio para Mujeres Víctimas de Violencia en el Instituto Hidalguense de las Mujeres.</t>
   </si>
 </sst>
 </file>
@@ -1484,7 +1498,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1580,6 +1594,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2377,35 +2395,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC10AE24-34E8-42A8-B125-F7B603DBE80A}">
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.81640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="32.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="35.1796875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="14.26953125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="36.453125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="25.81640625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="11.453125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="11.453125" style="1"/>
+    <col min="1" max="1" width="35.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="32.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="36.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="25.85546875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>139</v>
       </c>
@@ -2446,16 +2465,19 @@
         <v>3</v>
       </c>
       <c r="N1" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>290</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>140</v>
       </c>
@@ -2495,21 +2517,24 @@
       <c r="M2" s="3">
         <v>68143</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="P2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="21" t="e" vm="1">
-        <f>_xlfn.IMAGE(Q2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q2" s="7" t="s">
+      <c r="Q2" s="21" t="e" vm="1">
+        <f>_xlfn.IMAGE(R2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R2" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>141</v>
       </c>
@@ -2549,21 +2574,22 @@
       <c r="M3" s="3">
         <v>61122</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="3"/>
+      <c r="O3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="P3" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="P3" s="21" t="e" vm="2">
-        <f>_xlfn.IMAGE(Q3)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="21" t="e" vm="2">
+        <f>_xlfn.IMAGE(R3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>142</v>
       </c>
@@ -2603,21 +2629,22 @@
       <c r="M4" s="3">
         <v>61818</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="3"/>
+      <c r="O4" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="P4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="P4" s="21" t="e" vm="3">
-        <f>_xlfn.IMAGE(Q4)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q4" s="1" t="s">
+      <c r="Q4" s="21" t="e" vm="3">
+        <f>_xlfn.IMAGE(R4)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R4" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>143</v>
       </c>
@@ -2657,21 +2684,22 @@
       <c r="M5" s="3">
         <v>61482</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="N5" s="3"/>
+      <c r="O5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="O5" s="11" t="s">
+      <c r="P5" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P5" s="21" t="e" vm="4">
-        <f>_xlfn.IMAGE(Q5)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" s="21" t="e" vm="4">
+        <f>_xlfn.IMAGE(R5)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R5" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>144</v>
       </c>
@@ -2711,21 +2739,22 @@
       <c r="M6" s="3">
         <v>67882</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="N6" s="3"/>
+      <c r="O6" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="P6" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="P6" s="21" t="e" vm="5">
-        <f>_xlfn.IMAGE(Q6)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6" s="21" t="e" vm="5">
+        <f>_xlfn.IMAGE(R6)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R6" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>145</v>
       </c>
@@ -2765,21 +2794,22 @@
       <c r="M7" s="15">
         <v>61514</v>
       </c>
-      <c r="N7" s="16" t="s">
+      <c r="N7" s="15"/>
+      <c r="O7" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="O7" s="23" t="s">
+      <c r="P7" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="P7" s="24" t="e" vm="6">
-        <f t="shared" ref="P7:P19" si="0">_xlfn.IMAGE(Q7)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" s="24" t="e" vm="6">
+        <f t="shared" ref="Q7:Q19" si="0">_xlfn.IMAGE(R7)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R7" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>146</v>
       </c>
@@ -2819,21 +2849,22 @@
       <c r="M8" s="3">
         <v>61266</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="N8" s="3"/>
+      <c r="O8" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="O8" s="11" t="s">
+      <c r="P8" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="P8" s="21" t="e" vm="7">
+      <c r="Q8" s="21" t="e" vm="7">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>53</v>
       </c>
@@ -2873,21 +2904,22 @@
       <c r="M9" s="3">
         <v>61442</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="N9" s="3"/>
+      <c r="O9" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="O9" s="11" t="s">
+      <c r="P9" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="P9" s="21" t="e" vm="8">
+      <c r="Q9" s="21" t="e" vm="8">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="R9" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>147</v>
       </c>
@@ -2927,21 +2959,22 @@
       <c r="M10" s="3">
         <v>59911</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="N10" s="3"/>
+      <c r="O10" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="O10" s="11" t="s">
+      <c r="P10" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="P10" s="21" t="e" vm="9">
+      <c r="Q10" s="21" t="e" vm="9">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="R10" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>148</v>
       </c>
@@ -2981,21 +3014,22 @@
       <c r="M11" s="3">
         <v>59098</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="N11" s="3"/>
+      <c r="O11" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="O11" s="11" t="s">
+      <c r="P11" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="P11" s="21" t="e" vm="10">
+      <c r="Q11" s="21" t="e" vm="10">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="R11" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>149</v>
       </c>
@@ -3035,21 +3069,22 @@
       <c r="M12" s="3">
         <v>62036</v>
       </c>
-      <c r="N12" s="5" t="s">
+      <c r="N12" s="3"/>
+      <c r="O12" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="O12" s="11" t="s">
+      <c r="P12" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="P12" s="21" t="e" vm="11">
+      <c r="Q12" s="21" t="e" vm="11">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="R12" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>150</v>
       </c>
@@ -3089,21 +3124,22 @@
       <c r="M13" s="3">
         <v>59457</v>
       </c>
-      <c r="N13" s="5" t="s">
+      <c r="N13" s="3"/>
+      <c r="O13" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="O13" s="11" t="s">
+      <c r="P13" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="P13" s="21" t="e" vm="12">
+      <c r="Q13" s="21" t="e" vm="12">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="Q13" s="1" t="s">
+      <c r="R13" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>151</v>
       </c>
@@ -3143,21 +3179,22 @@
       <c r="M14" s="3">
         <v>62616</v>
       </c>
-      <c r="N14" s="5" t="s">
+      <c r="N14" s="3"/>
+      <c r="O14" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="O14" s="11" t="s">
+      <c r="P14" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="P14" s="21" t="e" vm="13">
+      <c r="Q14" s="21" t="e" vm="13">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="Q14" s="1" t="s">
+      <c r="R14" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>152</v>
       </c>
@@ -3197,21 +3234,22 @@
       <c r="M15" s="3">
         <v>61440</v>
       </c>
-      <c r="N15" s="5" t="s">
+      <c r="N15" s="3"/>
+      <c r="O15" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="O15" s="11" t="s">
+      <c r="P15" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="P15" s="21" t="e" vm="14">
+      <c r="Q15" s="21" t="e" vm="14">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="Q15" s="1" t="s">
+      <c r="R15" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>153</v>
       </c>
@@ -3251,21 +3289,22 @@
       <c r="M16" s="3">
         <v>67850</v>
       </c>
-      <c r="N16" s="6" t="s">
+      <c r="N16" s="3"/>
+      <c r="O16" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="O16" s="12" t="s">
+      <c r="P16" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="P16" s="21" t="e" vm="15">
+      <c r="Q16" s="21" t="e" vm="15">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="Q16" s="1" t="s">
+      <c r="R16" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>154</v>
       </c>
@@ -3305,21 +3344,22 @@
       <c r="M17" s="3">
         <v>59885</v>
       </c>
-      <c r="N17" s="6" t="s">
+      <c r="N17" s="3"/>
+      <c r="O17" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="O17" s="12" t="s">
+      <c r="P17" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="P17" s="21" t="e" vm="16">
+      <c r="Q17" s="21" t="e" vm="16">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="Q17" s="1" t="s">
+      <c r="R17" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>155</v>
       </c>
@@ -3359,21 +3399,22 @@
       <c r="M18" s="3">
         <v>62028</v>
       </c>
-      <c r="N18" s="5" t="s">
+      <c r="N18" s="3"/>
+      <c r="O18" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="O18" s="12" t="s">
+      <c r="P18" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="P18" s="21" t="e" vm="17">
+      <c r="Q18" s="21" t="e" vm="17">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="Q18" s="1" t="s">
+      <c r="R18" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>156</v>
       </c>
@@ -3413,21 +3454,22 @@
       <c r="M19" s="3">
         <v>62102</v>
       </c>
-      <c r="N19" s="6" t="s">
+      <c r="N19" s="3"/>
+      <c r="O19" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="O19" s="12" t="s">
+      <c r="P19" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="P19" s="21" t="e" vm="18">
+      <c r="Q19" s="21" t="e" vm="18">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="Q19" s="1" t="s">
+      <c r="R19" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>157</v>
       </c>
@@ -3467,21 +3509,22 @@
       <c r="M20" s="18">
         <v>55114</v>
       </c>
-      <c r="N20" s="19" t="s">
+      <c r="N20" s="18"/>
+      <c r="O20" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="O20" s="20" t="s">
+      <c r="P20" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="P20" s="25" t="e" vm="19">
-        <f>_xlfn.IMAGE(Q20)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q20" s="1" t="s">
+      <c r="Q20" s="25" t="e" vm="19">
+        <f>_xlfn.IMAGE(R20)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R20" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>291</v>
       </c>
@@ -3519,21 +3562,22 @@
       <c r="M21" s="21">
         <v>61486</v>
       </c>
-      <c r="N21" s="26" t="s">
+      <c r="N21" s="21"/>
+      <c r="O21" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="O21" s="26" t="s">
+      <c r="P21" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="P21" s="21" t="e" vm="20">
-        <f>_xlfn.IMAGE(Q21)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q21" s="1" t="s">
+      <c r="Q21" s="21" t="e" vm="20">
+        <f>_xlfn.IMAGE(R21)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R21" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>292</v>
       </c>
@@ -3571,72 +3615,1214 @@
       <c r="M22" s="21">
         <v>61595</v>
       </c>
-      <c r="N22" s="26" t="s">
+      <c r="N22" s="21"/>
+      <c r="O22" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="O22" s="26" t="s">
+      <c r="P22" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="P22" s="21" t="e" vm="21">
-        <f>_xlfn.IMAGE(Q22)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q22" s="1" t="s">
+      <c r="Q22" s="21" t="e" vm="21">
+        <f>_xlfn.IMAGE(R22)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R22" s="1" t="s">
         <v>169</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1" xr:uid="{5B45C678-22C4-4527-9B36-CB8D21A82B62}"/>
-    <hyperlink ref="O2" r:id="rId2" xr:uid="{FB100B36-3BDB-4D08-BE77-29E0240C9C0D}"/>
-    <hyperlink ref="Q2" r:id="rId3" xr:uid="{BC47187C-CD2A-4855-A1BB-FE32F5D2D380}"/>
-    <hyperlink ref="N3" r:id="rId4" xr:uid="{09E71C77-DAF0-451F-B2DA-51FCE9E753FD}"/>
-    <hyperlink ref="O3" r:id="rId5" xr:uid="{071B46E0-1331-4BA8-AE95-5449B6AC9598}"/>
-    <hyperlink ref="O4" r:id="rId6" xr:uid="{CDEA95C9-D2DD-4E1C-9B79-64FE828B11C1}"/>
-    <hyperlink ref="N4" r:id="rId7" xr:uid="{ECD4C629-5BE5-4061-9C0E-4224EC90E3E7}"/>
-    <hyperlink ref="N5" r:id="rId8" xr:uid="{192B940F-9CB5-485B-84E9-DC801E1B3C54}"/>
-    <hyperlink ref="O5" r:id="rId9" xr:uid="{AEB812B4-3099-48CD-AA77-6E7738BA5F2B}"/>
-    <hyperlink ref="O6" r:id="rId10" xr:uid="{317FFB50-C85A-4037-827B-E5E5435C6620}"/>
-    <hyperlink ref="N6" r:id="rId11" xr:uid="{E74EBE2A-332D-4D1B-82D8-4899328E7CC2}"/>
-    <hyperlink ref="N7" r:id="rId12" xr:uid="{88234E48-A477-4311-AE76-C2E7C4D4F265}"/>
-    <hyperlink ref="O7" r:id="rId13" xr:uid="{731F08ED-728A-455E-8549-4AFA35594F0A}"/>
-    <hyperlink ref="N8" r:id="rId14" xr:uid="{91DDF47F-E44B-4A33-B31A-FAD99EF8CBC9}"/>
-    <hyperlink ref="O8" r:id="rId15" xr:uid="{B2F2F329-8F0B-4596-8B27-F3BF6C8E0204}"/>
-    <hyperlink ref="O9" r:id="rId16" xr:uid="{08CE1C0B-73D0-42F6-8AD9-5D27E165B0F2}"/>
-    <hyperlink ref="N9" r:id="rId17" xr:uid="{F4D8EB26-286B-4AC8-A3AE-7B28FF0E911F}"/>
-    <hyperlink ref="O10" r:id="rId18" xr:uid="{79C40CC4-ED6C-466E-97D5-427D447B038A}"/>
-    <hyperlink ref="N10" r:id="rId19" xr:uid="{411E7C96-FFF7-476D-BEBE-EFA5179E54CE}"/>
-    <hyperlink ref="N11" r:id="rId20" xr:uid="{ECF41EB3-3D43-4EE8-9F36-3AAF7225FEE7}"/>
-    <hyperlink ref="O11" r:id="rId21" xr:uid="{5A09DE2C-B90D-45EE-83A6-1AC64FAF2031}"/>
-    <hyperlink ref="O12" r:id="rId22" xr:uid="{A083B4D6-643A-4FB5-B3ED-F615FBE13CC7}"/>
-    <hyperlink ref="N12" r:id="rId23" xr:uid="{727D39E6-798C-418B-9EC2-E22B25756084}"/>
-    <hyperlink ref="N13" r:id="rId24" xr:uid="{9B42C4D8-5B2B-44E8-88A3-657564F737D3}"/>
-    <hyperlink ref="O13" r:id="rId25" xr:uid="{1F2C4431-9AEA-41F5-A7C4-53D6CDAAC4D3}"/>
-    <hyperlink ref="O14" r:id="rId26" xr:uid="{DC74FC01-C676-4F03-9146-E55C96B74393}"/>
-    <hyperlink ref="N14" r:id="rId27" xr:uid="{AE83C712-8225-411D-880D-1659BE6C9703}"/>
-    <hyperlink ref="O15" r:id="rId28" xr:uid="{F36BF8FE-451C-4445-9EBA-A34F27BBB3E1}"/>
-    <hyperlink ref="N15" r:id="rId29" xr:uid="{72F27100-8E90-4921-B73F-4BC79E7F4389}"/>
-    <hyperlink ref="N16" r:id="rId30" xr:uid="{6093E294-459B-47FA-86F4-BCD268E886E8}"/>
-    <hyperlink ref="O16" r:id="rId31" xr:uid="{17D4B546-1B5E-4440-B018-ABC61059B712}"/>
-    <hyperlink ref="N17" r:id="rId32" xr:uid="{95EE1CB3-A7F0-46DB-81B5-CB93D6B5F617}"/>
-    <hyperlink ref="O17" r:id="rId33" xr:uid="{76A8C8B6-BEF4-481C-A2AE-C0A36977C760}"/>
-    <hyperlink ref="O18" r:id="rId34" xr:uid="{DD790A20-D93D-4AC9-9943-60327D97FB4E}"/>
-    <hyperlink ref="N18" r:id="rId35" xr:uid="{8B565906-3090-431F-98A0-4A19F057AB83}"/>
-    <hyperlink ref="N19" r:id="rId36" xr:uid="{68440965-FBE0-4D22-B28B-C72EA7D75DBC}"/>
-    <hyperlink ref="O19" r:id="rId37" xr:uid="{2569B8A3-1DBA-46B2-8F2E-0CFB569C1680}"/>
-    <hyperlink ref="O20" r:id="rId38" xr:uid="{AFB19B82-D5C2-4D02-B436-C7CAF036799F}"/>
-    <hyperlink ref="N20" r:id="rId39" xr:uid="{32EB2C30-C8A3-4312-84DB-F3F377C165C2}"/>
-    <hyperlink ref="N21" r:id="rId40" xr:uid="{59AC364B-0371-4893-B57B-94CD733E1A8D}"/>
-    <hyperlink ref="O21" r:id="rId41" location="PerfiLegislador%20zoraya.villacis@diputados.gob.mx" xr:uid="{F4C58A32-8684-4C31-B867-CEE1E236BCAF}"/>
-    <hyperlink ref="N22" r:id="rId42" xr:uid="{D5C0B0D7-36CC-43B7-B14B-4337F2C9FFBB}"/>
-    <hyperlink ref="O22" r:id="rId43" xr:uid="{D7D55FB6-9C2F-41F8-877D-5193136850A2}"/>
+    <hyperlink ref="O2" r:id="rId1" xr:uid="{5B45C678-22C4-4527-9B36-CB8D21A82B62}"/>
+    <hyperlink ref="P2" r:id="rId2" xr:uid="{FB100B36-3BDB-4D08-BE77-29E0240C9C0D}"/>
+    <hyperlink ref="R2" r:id="rId3" xr:uid="{BC47187C-CD2A-4855-A1BB-FE32F5D2D380}"/>
+    <hyperlink ref="O3" r:id="rId4" xr:uid="{09E71C77-DAF0-451F-B2DA-51FCE9E753FD}"/>
+    <hyperlink ref="P3" r:id="rId5" xr:uid="{071B46E0-1331-4BA8-AE95-5449B6AC9598}"/>
+    <hyperlink ref="P4" r:id="rId6" xr:uid="{CDEA95C9-D2DD-4E1C-9B79-64FE828B11C1}"/>
+    <hyperlink ref="O4" r:id="rId7" xr:uid="{ECD4C629-5BE5-4061-9C0E-4224EC90E3E7}"/>
+    <hyperlink ref="O5" r:id="rId8" xr:uid="{192B940F-9CB5-485B-84E9-DC801E1B3C54}"/>
+    <hyperlink ref="P5" r:id="rId9" xr:uid="{AEB812B4-3099-48CD-AA77-6E7738BA5F2B}"/>
+    <hyperlink ref="P6" r:id="rId10" xr:uid="{317FFB50-C85A-4037-827B-E5E5435C6620}"/>
+    <hyperlink ref="O6" r:id="rId11" xr:uid="{E74EBE2A-332D-4D1B-82D8-4899328E7CC2}"/>
+    <hyperlink ref="O7" r:id="rId12" xr:uid="{88234E48-A477-4311-AE76-C2E7C4D4F265}"/>
+    <hyperlink ref="P7" r:id="rId13" xr:uid="{731F08ED-728A-455E-8549-4AFA35594F0A}"/>
+    <hyperlink ref="O8" r:id="rId14" xr:uid="{91DDF47F-E44B-4A33-B31A-FAD99EF8CBC9}"/>
+    <hyperlink ref="P8" r:id="rId15" xr:uid="{B2F2F329-8F0B-4596-8B27-F3BF6C8E0204}"/>
+    <hyperlink ref="P9" r:id="rId16" xr:uid="{08CE1C0B-73D0-42F6-8AD9-5D27E165B0F2}"/>
+    <hyperlink ref="O9" r:id="rId17" xr:uid="{F4D8EB26-286B-4AC8-A3AE-7B28FF0E911F}"/>
+    <hyperlink ref="P10" r:id="rId18" xr:uid="{79C40CC4-ED6C-466E-97D5-427D447B038A}"/>
+    <hyperlink ref="O10" r:id="rId19" xr:uid="{411E7C96-FFF7-476D-BEBE-EFA5179E54CE}"/>
+    <hyperlink ref="O11" r:id="rId20" xr:uid="{ECF41EB3-3D43-4EE8-9F36-3AAF7225FEE7}"/>
+    <hyperlink ref="P11" r:id="rId21" xr:uid="{5A09DE2C-B90D-45EE-83A6-1AC64FAF2031}"/>
+    <hyperlink ref="P12" r:id="rId22" xr:uid="{A083B4D6-643A-4FB5-B3ED-F615FBE13CC7}"/>
+    <hyperlink ref="O12" r:id="rId23" xr:uid="{727D39E6-798C-418B-9EC2-E22B25756084}"/>
+    <hyperlink ref="O13" r:id="rId24" xr:uid="{9B42C4D8-5B2B-44E8-88A3-657564F737D3}"/>
+    <hyperlink ref="P13" r:id="rId25" xr:uid="{1F2C4431-9AEA-41F5-A7C4-53D6CDAAC4D3}"/>
+    <hyperlink ref="P14" r:id="rId26" xr:uid="{DC74FC01-C676-4F03-9146-E55C96B74393}"/>
+    <hyperlink ref="O14" r:id="rId27" xr:uid="{AE83C712-8225-411D-880D-1659BE6C9703}"/>
+    <hyperlink ref="P15" r:id="rId28" xr:uid="{F36BF8FE-451C-4445-9EBA-A34F27BBB3E1}"/>
+    <hyperlink ref="O15" r:id="rId29" xr:uid="{72F27100-8E90-4921-B73F-4BC79E7F4389}"/>
+    <hyperlink ref="O16" r:id="rId30" xr:uid="{6093E294-459B-47FA-86F4-BCD268E886E8}"/>
+    <hyperlink ref="P16" r:id="rId31" xr:uid="{17D4B546-1B5E-4440-B018-ABC61059B712}"/>
+    <hyperlink ref="O17" r:id="rId32" xr:uid="{95EE1CB3-A7F0-46DB-81B5-CB93D6B5F617}"/>
+    <hyperlink ref="P17" r:id="rId33" xr:uid="{76A8C8B6-BEF4-481C-A2AE-C0A36977C760}"/>
+    <hyperlink ref="P18" r:id="rId34" xr:uid="{DD790A20-D93D-4AC9-9943-60327D97FB4E}"/>
+    <hyperlink ref="O18" r:id="rId35" xr:uid="{8B565906-3090-431F-98A0-4A19F057AB83}"/>
+    <hyperlink ref="O19" r:id="rId36" xr:uid="{68440965-FBE0-4D22-B28B-C72EA7D75DBC}"/>
+    <hyperlink ref="P19" r:id="rId37" xr:uid="{2569B8A3-1DBA-46B2-8F2E-0CFB569C1680}"/>
+    <hyperlink ref="P20" r:id="rId38" xr:uid="{AFB19B82-D5C2-4D02-B436-C7CAF036799F}"/>
+    <hyperlink ref="O20" r:id="rId39" xr:uid="{32EB2C30-C8A3-4312-84DB-F3F377C165C2}"/>
+    <hyperlink ref="O21" r:id="rId40" xr:uid="{59AC364B-0371-4893-B57B-94CD733E1A8D}"/>
+    <hyperlink ref="P21" r:id="rId41" location="PerfiLegislador%20zoraya.villacis@diputados.gob.mx" xr:uid="{F4C58A32-8684-4C31-B867-CEE1E236BCAF}"/>
+    <hyperlink ref="O22" r:id="rId42" xr:uid="{D5C0B0D7-36CC-43B7-B14B-4337F2C9FFBB}"/>
+    <hyperlink ref="P22" r:id="rId43" xr:uid="{D7D55FB6-9C2F-41F8-877D-5193136850A2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{602D7C26-B72E-4BDF-8A11-ED95CDF1C662}">
+  <dimension ref="A1:R19"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" customWidth="1"/>
+    <col min="15" max="15" width="34.5703125" customWidth="1"/>
+    <col min="16" max="16" width="36.140625" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2" s="30">
+        <v>45518</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="30">
+        <v>44437</v>
+      </c>
+      <c r="G2" s="30">
+        <v>45535</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="L2" s="22">
+        <v>5550360000</v>
+      </c>
+      <c r="M2" s="22">
+        <v>59864</v>
+      </c>
+      <c r="N2" s="22"/>
+      <c r="O2" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="P2" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q2" s="22" t="e" vm="22">
+        <f>_xlfn.IMAGE(R2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R2" s="33" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>264</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="27">
+        <v>45601</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="F3" s="30">
+        <v>44437</v>
+      </c>
+      <c r="G3" s="30">
+        <v>46630</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="L3" s="22">
+        <v>5550360000</v>
+      </c>
+      <c r="M3" s="22">
+        <v>61533</v>
+      </c>
+      <c r="N3" s="22"/>
+      <c r="O3" s="26" t="s">
+        <v>179</v>
+      </c>
+      <c r="P3" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q3" s="22" t="e" vm="23">
+        <f t="shared" ref="Q3:Q19" si="0">_xlfn.IMAGE(R3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R3" s="33" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="C4" s="30">
+        <v>45595</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="F4" s="30">
+        <v>44437</v>
+      </c>
+      <c r="G4" s="30">
+        <v>46630</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="L4" s="22">
+        <v>5550360000</v>
+      </c>
+      <c r="M4" s="22">
+        <v>61460</v>
+      </c>
+      <c r="N4" s="22"/>
+      <c r="O4" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="P4" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q4" s="22" t="e" vm="24">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R4" s="33" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="C5" s="30">
+        <v>45601</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="F5" s="30">
+        <v>44437</v>
+      </c>
+      <c r="G5" s="30">
+        <v>46630</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="L5" s="22">
+        <v>5550360000</v>
+      </c>
+      <c r="M5" s="22">
+        <v>61822</v>
+      </c>
+      <c r="N5" s="22"/>
+      <c r="O5" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="P5" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q5" s="22" t="e" vm="25">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R5" s="33" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>267</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="C6" s="30">
+        <v>45595</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="F6" s="30">
+        <v>44437</v>
+      </c>
+      <c r="G6" s="30">
+        <v>46630</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="L6" s="22">
+        <v>5550360000</v>
+      </c>
+      <c r="M6" s="22">
+        <v>61498</v>
+      </c>
+      <c r="N6" s="22"/>
+      <c r="O6" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="P6" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q6" s="22" t="e" vm="26">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R6" s="33" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>268</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="30">
+        <v>44476</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="30">
+        <v>44437</v>
+      </c>
+      <c r="G7" s="30">
+        <v>46630</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="L7" s="22">
+        <v>5550360000</v>
+      </c>
+      <c r="M7" s="22">
+        <v>61841</v>
+      </c>
+      <c r="N7" s="22"/>
+      <c r="O7" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="P7" s="34" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q7" s="22" t="e" vm="27">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R7" s="33" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="C8" s="30">
+        <v>45595</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="F8" s="30">
+        <v>44437</v>
+      </c>
+      <c r="G8" s="30">
+        <v>46630</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="L8" s="22">
+        <v>5550360000</v>
+      </c>
+      <c r="M8" s="22">
+        <v>61474</v>
+      </c>
+      <c r="N8" s="22"/>
+      <c r="O8" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="P8" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q8" s="22" t="e" vm="28">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R8" s="33" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>270</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="F9" s="30">
+        <v>44437</v>
+      </c>
+      <c r="G9" s="30">
+        <v>46630</v>
+      </c>
+      <c r="H9" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="J9" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K9" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="L9" s="22">
+        <v>5550360000</v>
+      </c>
+      <c r="M9" s="22">
+        <v>67881</v>
+      </c>
+      <c r="N9" s="22"/>
+      <c r="O9" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="P9" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q9" s="22" t="e" vm="29">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R9" s="33" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="30">
+        <v>45595</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="F10" s="30">
+        <v>44437</v>
+      </c>
+      <c r="G10" s="30">
+        <v>46630</v>
+      </c>
+      <c r="H10" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="J10" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="L10" s="22">
+        <v>5550360000</v>
+      </c>
+      <c r="M10" s="22">
+        <v>61372</v>
+      </c>
+      <c r="N10" s="22"/>
+      <c r="O10" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="P10" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q10" s="22" t="e" vm="30">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R10" s="33" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>272</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="F11" s="30">
+        <v>44437</v>
+      </c>
+      <c r="G11" s="30">
+        <v>46630</v>
+      </c>
+      <c r="H11" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="L11" s="22">
+        <v>5550360000</v>
+      </c>
+      <c r="M11" s="22">
+        <v>61629</v>
+      </c>
+      <c r="N11" s="22"/>
+      <c r="O11" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="P11" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q11" s="22" t="e" vm="31">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R11" s="33" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="30">
+        <v>45595</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="F12" s="30">
+        <v>44437</v>
+      </c>
+      <c r="G12" s="30">
+        <v>46630</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="J12" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K12" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="L12" s="22">
+        <v>5550360000</v>
+      </c>
+      <c r="M12" s="22">
+        <v>59889</v>
+      </c>
+      <c r="N12" s="22"/>
+      <c r="O12" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="P12" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q12" s="22" t="e" vm="32">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R12" s="33" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>274</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="30">
+        <v>45595</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="F13" s="30">
+        <v>44437</v>
+      </c>
+      <c r="G13" s="30">
+        <v>46630</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="J13" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K13" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="L13" s="22">
+        <v>5550360000</v>
+      </c>
+      <c r="M13" s="22">
+        <v>59914</v>
+      </c>
+      <c r="N13" s="22"/>
+      <c r="O13" s="26" t="s">
+        <v>230</v>
+      </c>
+      <c r="P13" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q13" s="22" t="e" vm="33">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R13" s="33" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>275</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="30">
+        <v>45595</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="F14" s="30">
+        <v>44437</v>
+      </c>
+      <c r="G14" s="30">
+        <v>46630</v>
+      </c>
+      <c r="H14" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="J14" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K14" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="L14" s="22">
+        <v>5550360000</v>
+      </c>
+      <c r="M14" s="22">
+        <v>59918</v>
+      </c>
+      <c r="N14" s="22"/>
+      <c r="O14" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="P14" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q14" s="22" t="e" vm="34">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R14" s="33" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>276</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="30">
+        <v>45595</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="F15" s="30">
+        <v>44437</v>
+      </c>
+      <c r="G15" s="30">
+        <v>46630</v>
+      </c>
+      <c r="H15" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="J15" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K15" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="L15" s="22">
+        <v>5550360000</v>
+      </c>
+      <c r="M15" s="22">
+        <v>62067</v>
+      </c>
+      <c r="N15" s="22"/>
+      <c r="O15" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="P15" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q15" s="22" t="e" vm="35">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R15" s="33" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
+        <v>277</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="30">
+        <v>44437</v>
+      </c>
+      <c r="G16" s="30">
+        <v>46630</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="J16" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K16" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="L16" s="22">
+        <v>5550360000</v>
+      </c>
+      <c r="M16" s="22">
+        <v>62054</v>
+      </c>
+      <c r="N16" s="22"/>
+      <c r="O16" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="P16" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q16" s="22" t="e" vm="36">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R16" s="33" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="C17" s="30">
+        <v>45595</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="F17" s="30">
+        <v>44437</v>
+      </c>
+      <c r="G17" s="30">
+        <v>46630</v>
+      </c>
+      <c r="H17" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="J17" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K17" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="L17" s="22">
+        <v>5550360000</v>
+      </c>
+      <c r="M17" s="22">
+        <v>62636</v>
+      </c>
+      <c r="N17" s="22"/>
+      <c r="O17" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="P17" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q17" s="22" t="e" vm="37">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R17" s="33" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="30">
+        <v>45595</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="F18" s="30">
+        <v>44437</v>
+      </c>
+      <c r="G18" s="30">
+        <v>46630</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="I18" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="J18" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K18" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="L18" s="22">
+        <v>5550360000</v>
+      </c>
+      <c r="M18" s="22">
+        <v>59410</v>
+      </c>
+      <c r="N18" s="22"/>
+      <c r="O18" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="P18" s="26" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q18" s="22" t="e" vm="38">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R18" s="33" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="30">
+        <v>45595</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="F19" s="30">
+        <v>44437</v>
+      </c>
+      <c r="G19" s="30">
+        <v>46630</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="I19" s="22" t="s">
+        <v>258</v>
+      </c>
+      <c r="J19" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K19" s="22" t="s">
+        <v>259</v>
+      </c>
+      <c r="L19" s="22">
+        <v>5550360000</v>
+      </c>
+      <c r="M19" s="22">
+        <v>68850</v>
+      </c>
+      <c r="N19" s="22"/>
+      <c r="O19" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="P19" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q19" s="22" t="e" vm="39">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R19" s="33" t="s">
+        <v>262</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="O2" r:id="rId1" xr:uid="{F494D8B1-27C6-49D3-8FDD-9A4396888437}"/>
+    <hyperlink ref="P2" r:id="rId2" display="https://sil.gobernacion.gob.mx/Librerias/pp_PerfilLegislador.php?Referencia=9227697" xr:uid="{5B19A580-883E-4B41-9303-21D9AB3641A7}"/>
+    <hyperlink ref="O3" r:id="rId3" xr:uid="{F1388137-65F9-4252-86D9-E7597A1DD03E}"/>
+    <hyperlink ref="P3" r:id="rId4" xr:uid="{5FEE3462-39AB-4EAF-8369-BE80C65E4B90}"/>
+    <hyperlink ref="O4" r:id="rId5" xr:uid="{BBC9461B-0678-411D-B47B-4D1E0EDA5BEF}"/>
+    <hyperlink ref="P4" r:id="rId6" xr:uid="{1815E2D8-2F71-4519-BE39-579D298E3A16}"/>
+    <hyperlink ref="K5" r:id="rId7" xr:uid="{E703AEC8-8E73-4F2A-A17B-1DF7A9E31FDC}"/>
+    <hyperlink ref="O5" r:id="rId8" xr:uid="{0E9EF265-D266-4B65-BF58-2CCD8CC9AACB}"/>
+    <hyperlink ref="P5" r:id="rId9" xr:uid="{5DB6F1C2-79A4-4181-A13A-110DFFAA4D9A}"/>
+    <hyperlink ref="O6" r:id="rId10" xr:uid="{41E8213E-4E3A-4D42-A6BD-0366D39EF74D}"/>
+    <hyperlink ref="P6" r:id="rId11" xr:uid="{82B296D6-8208-4E63-8C9E-1F73B030A4C1}"/>
+    <hyperlink ref="K6" r:id="rId12" xr:uid="{5E2229D4-4652-4AA0-A2B1-388066D5E992}"/>
+    <hyperlink ref="K7" r:id="rId13" xr:uid="{8C40449E-2EBF-4901-B172-1161B5845D72}"/>
+    <hyperlink ref="O7" r:id="rId14" xr:uid="{DF390B30-8E75-496E-B3C6-92B6CABB737B}"/>
+    <hyperlink ref="P7" r:id="rId15" xr:uid="{E32EBEB0-8F27-4EA2-9850-29C1DE3145B2}"/>
+    <hyperlink ref="K8" r:id="rId16" xr:uid="{165CFDFC-5DE9-4941-9AFA-7C473A4B4454}"/>
+    <hyperlink ref="O8" r:id="rId17" xr:uid="{00AF7454-AFD7-4366-AC95-35870231087F}"/>
+    <hyperlink ref="P8" r:id="rId18" xr:uid="{80BD1492-DB63-4558-83F3-1C4EF72F8FC9}"/>
+    <hyperlink ref="K9" r:id="rId19" xr:uid="{A1A3E78F-48C4-4EED-8843-00F80EFD0937}"/>
+    <hyperlink ref="O9" r:id="rId20" xr:uid="{AE92BE08-5DCE-43F1-9BDF-790B2864E8DD}"/>
+    <hyperlink ref="P9" r:id="rId21" xr:uid="{D185C4FB-45FE-44B7-B513-16E611CC42C2}"/>
+    <hyperlink ref="K10" r:id="rId22" xr:uid="{C3D291B8-CD03-404D-B656-FFE8C257F9C0}"/>
+    <hyperlink ref="O10" r:id="rId23" xr:uid="{82AC9C62-8987-4D28-971D-FBDAEBC5A597}"/>
+    <hyperlink ref="P10" r:id="rId24" xr:uid="{ABCC48D5-E5D2-4BC0-B0A5-04198F7F8AD0}"/>
+    <hyperlink ref="O11" r:id="rId25" xr:uid="{69B211E6-239D-48D7-8D88-F7E2991CBE8C}"/>
+    <hyperlink ref="P11" r:id="rId26" xr:uid="{6555C734-4D37-49E4-A153-0C776E9B84B4}"/>
+    <hyperlink ref="O12" r:id="rId27" xr:uid="{106AE3DA-6EBF-43CF-BAE0-CD36A4658FDE}"/>
+    <hyperlink ref="P12" r:id="rId28" xr:uid="{DF775BD4-8237-47A7-9094-7AAC4D78AFF4}"/>
+    <hyperlink ref="O13" r:id="rId29" xr:uid="{ABB1B2ED-0A30-488B-8515-B66E02F1D1A4}"/>
+    <hyperlink ref="P13" r:id="rId30" xr:uid="{869870C5-5119-415F-9A07-CD39FAB22D56}"/>
+    <hyperlink ref="O14" r:id="rId31" xr:uid="{0E9AB998-45B2-4109-B4CF-D8BEB382A174}"/>
+    <hyperlink ref="P14" r:id="rId32" xr:uid="{4DC7DD20-9026-4B66-988E-23B823CB28EC}"/>
+    <hyperlink ref="O15" r:id="rId33" xr:uid="{994283AA-16AC-44C8-8780-AA7B390BF5C3}"/>
+    <hyperlink ref="P15" r:id="rId34" location="PerfiLegislador" xr:uid="{F7E818F6-85ED-41B4-A012-E2424A6F1FB9}"/>
+    <hyperlink ref="K16" r:id="rId35" xr:uid="{0D7A8C28-767C-48E9-B602-16C2E50CAC9B}"/>
+    <hyperlink ref="O16" r:id="rId36" xr:uid="{48A3ED08-0ECD-4DFD-8889-844FF9DA52B5}"/>
+    <hyperlink ref="P16" r:id="rId37" xr:uid="{7D368797-4789-4A79-92D6-201E097EC361}"/>
+    <hyperlink ref="K17" r:id="rId38" xr:uid="{D0F9196F-0A9D-4F69-8509-F1FEEB09E565}"/>
+    <hyperlink ref="O17" r:id="rId39" xr:uid="{0283BAB0-C844-44C5-B2F2-2E7127C0DCBF}"/>
+    <hyperlink ref="P17" r:id="rId40" xr:uid="{9B71341F-F7C9-4D0E-BC8E-E7E8F0CA1C75}"/>
+    <hyperlink ref="K18" r:id="rId41" xr:uid="{225E9022-C9CC-48E9-84D5-4AA8EADDE397}"/>
+    <hyperlink ref="O18" r:id="rId42" xr:uid="{1CFA5889-0439-4365-B00C-BB5521AF2CC0}"/>
+    <hyperlink ref="P18" r:id="rId43" xr:uid="{9CE466C4-AF07-4271-B133-56EA385BFC65}"/>
+    <hyperlink ref="O19" r:id="rId44" xr:uid="{1378D7C7-AAC3-4E37-A62B-F73A5997F15E}"/>
+    <hyperlink ref="P19" r:id="rId45" xr:uid="{F5C742A3-121F-48DE-87FF-BECBA6D75D75}"/>
+    <hyperlink ref="R2" r:id="rId46" xr:uid="{7AC39D02-ACC7-41D7-89C5-8344190DAD63}"/>
+    <hyperlink ref="R3" r:id="rId47" xr:uid="{8DBF2AC7-6C4F-401F-971F-11CCE812931A}"/>
+    <hyperlink ref="R4" r:id="rId48" xr:uid="{467BD20C-F8F6-4A4E-BAD2-1B61A85F33E7}"/>
+    <hyperlink ref="R5" r:id="rId49" xr:uid="{FE6792E6-C428-4B4C-8CFB-B32F3B12590B}"/>
+    <hyperlink ref="R6" r:id="rId50" xr:uid="{38D2D3BA-6A99-4125-9C92-B7B462579A1C}"/>
+    <hyperlink ref="R7" r:id="rId51" xr:uid="{BE3F65D3-6D17-4FA2-BF0C-00AEFDFFCDEE}"/>
+    <hyperlink ref="R8" r:id="rId52" xr:uid="{AD50E73D-6534-40C3-B550-A81AC6527633}"/>
+    <hyperlink ref="R9" r:id="rId53" xr:uid="{2D18B4A2-4EBF-4EA9-8CE1-1E4CFA15BBFC}"/>
+    <hyperlink ref="R10" r:id="rId54" xr:uid="{7ECEAC4A-2784-447B-BEA3-6D55A2D678B5}"/>
+    <hyperlink ref="R11" r:id="rId55" xr:uid="{4D8C64A5-1D68-46F6-BE83-9E28440B21E8}"/>
+    <hyperlink ref="R12" r:id="rId56" xr:uid="{B5BB0A16-41BC-4468-92B8-A4AFBCFDF0A0}"/>
+    <hyperlink ref="R13" r:id="rId57" xr:uid="{1D96DA6A-230D-4F51-A030-55872DD7F402}"/>
+    <hyperlink ref="R14" r:id="rId58" xr:uid="{73DD8F31-4840-48B9-83A2-8EDC30AD2ACD}"/>
+    <hyperlink ref="R15" r:id="rId59" xr:uid="{61054BB5-FBF8-4AF2-8A10-08C5A6525B17}"/>
+    <hyperlink ref="R16" r:id="rId60" xr:uid="{82822A1B-9515-498C-A092-33446564E761}"/>
+    <hyperlink ref="R17" r:id="rId61" xr:uid="{4C1F0D3C-5497-4C0A-83BD-40E979D5D440}"/>
+    <hyperlink ref="R18" r:id="rId62" xr:uid="{937267DF-6015-4779-8EDD-94FCE861FACA}"/>
+    <hyperlink ref="R19" r:id="rId63" xr:uid="{E8C9CE15-B54D-456F-A478-41EA4504FD5F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00029952-4CB9-454C-B0D3-5C1D0780C669}">
   <dimension ref="A1:G21"/>
   <sheetViews>
@@ -3644,16 +4830,16 @@
       <selection sqref="A1:G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.26953125" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>139</v>
       </c>
@@ -3674,7 +4860,7 @@
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>140</v>
       </c>
@@ -3698,7 +4884,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>141</v>
       </c>
@@ -3722,7 +4908,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>142</v>
       </c>
@@ -3746,7 +4932,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>143</v>
       </c>
@@ -3770,7 +4956,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>144</v>
       </c>
@@ -3794,7 +4980,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>146</v>
       </c>
@@ -3818,7 +5004,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>53</v>
       </c>
@@ -3842,7 +5028,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>147</v>
       </c>
@@ -3866,7 +5052,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>148</v>
       </c>
@@ -3890,7 +5076,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>149</v>
       </c>
@@ -3914,7 +5100,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>150</v>
       </c>
@@ -3938,7 +5124,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>151</v>
       </c>
@@ -3962,7 +5148,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>152</v>
       </c>
@@ -3986,7 +5172,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>153</v>
       </c>
@@ -4010,7 +5196,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>154</v>
       </c>
@@ -4034,7 +5220,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>155</v>
       </c>
@@ -4058,7 +5244,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>156</v>
       </c>
@@ -4082,7 +5268,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>157</v>
       </c>
@@ -4106,7 +5292,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>160</v>
       </c>
@@ -4130,7 +5316,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>165</v>
       </c>
@@ -4157,1107 +5343,6 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{063F9BD8-863B-45E8-975A-7D6A7FCCFF94}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{602D7C26-B72E-4BDF-8A11-ED95CDF1C662}">
-  <dimension ref="A1:Q19"/>
-  <sheetViews>
-    <sheetView topLeftCell="F14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="14.26953125" customWidth="1"/>
-    <col min="8" max="8" width="15.54296875" customWidth="1"/>
-    <col min="9" max="9" width="24.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="34.54296875" customWidth="1"/>
-    <col min="12" max="12" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.6328125" customWidth="1"/>
-    <col min="15" max="15" width="36.1796875" customWidth="1"/>
-    <col min="16" max="16" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.90625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="N1" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="P1" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="22" t="s">
-        <v>263</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="C2" s="30">
-        <v>45518</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="30">
-        <v>44437</v>
-      </c>
-      <c r="G2" s="30">
-        <v>45535</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>172</v>
-      </c>
-      <c r="L2" s="22">
-        <v>5550360000</v>
-      </c>
-      <c r="M2" s="22">
-        <v>59864</v>
-      </c>
-      <c r="N2" s="29" t="s">
-        <v>174</v>
-      </c>
-      <c r="O2" s="26" t="s">
-        <v>176</v>
-      </c>
-      <c r="P2" s="22" t="e" vm="22">
-        <f>_xlfn.IMAGE(Q2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="22" t="s">
-        <v>264</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="27">
-        <v>45601</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="F3" s="30">
-        <v>44437</v>
-      </c>
-      <c r="G3" s="30">
-        <v>46630</v>
-      </c>
-      <c r="H3" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="22" t="s">
-        <v>178</v>
-      </c>
-      <c r="J3" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="L3" s="22">
-        <v>5550360000</v>
-      </c>
-      <c r="M3" s="22">
-        <v>61533</v>
-      </c>
-      <c r="N3" s="26" t="s">
-        <v>179</v>
-      </c>
-      <c r="O3" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="P3" s="22" t="e" vm="23">
-        <f t="shared" ref="P3:P19" si="0">_xlfn.IMAGE(Q3)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="22" t="s">
-        <v>265</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>218</v>
-      </c>
-      <c r="C4" s="30">
-        <v>45595</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="F4" s="30">
-        <v>44437</v>
-      </c>
-      <c r="G4" s="30">
-        <v>46630</v>
-      </c>
-      <c r="H4" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="J4" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="L4" s="22">
-        <v>5550360000</v>
-      </c>
-      <c r="M4" s="22">
-        <v>61460</v>
-      </c>
-      <c r="N4" s="26" t="s">
-        <v>185</v>
-      </c>
-      <c r="O4" s="26" t="s">
-        <v>187</v>
-      </c>
-      <c r="P4" s="22" t="e" vm="24">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="22" t="s">
-        <v>266</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>218</v>
-      </c>
-      <c r="C5" s="30">
-        <v>45601</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="F5" s="30">
-        <v>44437</v>
-      </c>
-      <c r="G5" s="30">
-        <v>46630</v>
-      </c>
-      <c r="H5" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="J5" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="K5" s="26" t="s">
-        <v>189</v>
-      </c>
-      <c r="L5" s="22">
-        <v>5550360000</v>
-      </c>
-      <c r="M5" s="22">
-        <v>61822</v>
-      </c>
-      <c r="N5" s="26" t="s">
-        <v>190</v>
-      </c>
-      <c r="O5" s="26" t="s">
-        <v>191</v>
-      </c>
-      <c r="P5" s="22" t="e" vm="25">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="22" t="s">
-        <v>267</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>218</v>
-      </c>
-      <c r="C6" s="30">
-        <v>45595</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="F6" s="30">
-        <v>44437</v>
-      </c>
-      <c r="G6" s="30">
-        <v>46630</v>
-      </c>
-      <c r="H6" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="K6" s="26" t="s">
-        <v>195</v>
-      </c>
-      <c r="L6" s="22">
-        <v>5550360000</v>
-      </c>
-      <c r="M6" s="22">
-        <v>61498</v>
-      </c>
-      <c r="N6" s="26" t="s">
-        <v>193</v>
-      </c>
-      <c r="O6" s="26" t="s">
-        <v>194</v>
-      </c>
-      <c r="P6" s="22" t="e" vm="26">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="59" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="22" t="s">
-        <v>268</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="30">
-        <v>44476</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="30">
-        <v>44437</v>
-      </c>
-      <c r="G7" s="30">
-        <v>46630</v>
-      </c>
-      <c r="H7" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="I7" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="K7" s="26" t="s">
-        <v>197</v>
-      </c>
-      <c r="L7" s="22">
-        <v>5550360000</v>
-      </c>
-      <c r="M7" s="22">
-        <v>61841</v>
-      </c>
-      <c r="N7" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="O7" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="P7" s="22" t="e" vm="27">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="22" t="s">
-        <v>269</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>218</v>
-      </c>
-      <c r="C8" s="30">
-        <v>45595</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="F8" s="30">
-        <v>44437</v>
-      </c>
-      <c r="G8" s="30">
-        <v>46630</v>
-      </c>
-      <c r="H8" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="J8" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="K8" s="26" t="s">
-        <v>202</v>
-      </c>
-      <c r="L8" s="22">
-        <v>5550360000</v>
-      </c>
-      <c r="M8" s="22">
-        <v>61474</v>
-      </c>
-      <c r="N8" s="26" t="s">
-        <v>203</v>
-      </c>
-      <c r="O8" s="26" t="s">
-        <v>204</v>
-      </c>
-      <c r="P8" s="22" t="e" vm="28">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="22" t="s">
-        <v>270</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>206</v>
-      </c>
-      <c r="F9" s="30">
-        <v>44437</v>
-      </c>
-      <c r="G9" s="30">
-        <v>46630</v>
-      </c>
-      <c r="H9" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="J9" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="K9" s="26" t="s">
-        <v>208</v>
-      </c>
-      <c r="L9" s="22">
-        <v>5550360000</v>
-      </c>
-      <c r="M9" s="22">
-        <v>67881</v>
-      </c>
-      <c r="N9" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="O9" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="P9" s="22" t="e" vm="29">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="22" t="s">
-        <v>271</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="30">
-        <v>45595</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="F10" s="30">
-        <v>44437</v>
-      </c>
-      <c r="G10" s="30">
-        <v>46630</v>
-      </c>
-      <c r="H10" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="J10" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="K10" s="26" t="s">
-        <v>212</v>
-      </c>
-      <c r="L10" s="22">
-        <v>5550360000</v>
-      </c>
-      <c r="M10" s="22">
-        <v>61372</v>
-      </c>
-      <c r="N10" s="26" t="s">
-        <v>213</v>
-      </c>
-      <c r="O10" s="26" t="s">
-        <v>214</v>
-      </c>
-      <c r="P10" s="22" t="e" vm="30">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="22" t="s">
-        <v>272</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>218</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="F11" s="30">
-        <v>44437</v>
-      </c>
-      <c r="G11" s="30">
-        <v>46630</v>
-      </c>
-      <c r="H11" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="I11" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="K11" s="22" t="s">
-        <v>222</v>
-      </c>
-      <c r="L11" s="22">
-        <v>5550360000</v>
-      </c>
-      <c r="M11" s="22">
-        <v>61629</v>
-      </c>
-      <c r="N11" s="26" t="s">
-        <v>219</v>
-      </c>
-      <c r="O11" s="26" t="s">
-        <v>220</v>
-      </c>
-      <c r="P11" s="22" t="e" vm="31">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="22" t="s">
-        <v>273</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="30">
-        <v>45595</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="F12" s="30">
-        <v>44437</v>
-      </c>
-      <c r="G12" s="30">
-        <v>46630</v>
-      </c>
-      <c r="H12" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="22" t="s">
-        <v>223</v>
-      </c>
-      <c r="J12" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="K12" s="22" t="s">
-        <v>224</v>
-      </c>
-      <c r="L12" s="22">
-        <v>5550360000</v>
-      </c>
-      <c r="M12" s="22">
-        <v>59889</v>
-      </c>
-      <c r="N12" s="26" t="s">
-        <v>225</v>
-      </c>
-      <c r="O12" s="26" t="s">
-        <v>226</v>
-      </c>
-      <c r="P12" s="22" t="e" vm="32">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="22" t="s">
-        <v>274</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="30">
-        <v>45595</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="F13" s="30">
-        <v>44437</v>
-      </c>
-      <c r="G13" s="30">
-        <v>46630</v>
-      </c>
-      <c r="H13" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="J13" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="K13" s="22" t="s">
-        <v>229</v>
-      </c>
-      <c r="L13" s="22">
-        <v>5550360000</v>
-      </c>
-      <c r="M13" s="22">
-        <v>59914</v>
-      </c>
-      <c r="N13" s="26" t="s">
-        <v>230</v>
-      </c>
-      <c r="O13" s="26" t="s">
-        <v>231</v>
-      </c>
-      <c r="P13" s="22" t="e" vm="33">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="62" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="22" t="s">
-        <v>275</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="30">
-        <v>45595</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="F14" s="30">
-        <v>44437</v>
-      </c>
-      <c r="G14" s="30">
-        <v>46630</v>
-      </c>
-      <c r="H14" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="22" t="s">
-        <v>233</v>
-      </c>
-      <c r="J14" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="K14" s="22" t="s">
-        <v>234</v>
-      </c>
-      <c r="L14" s="22">
-        <v>5550360000</v>
-      </c>
-      <c r="M14" s="22">
-        <v>59918</v>
-      </c>
-      <c r="N14" s="26" t="s">
-        <v>235</v>
-      </c>
-      <c r="O14" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="P14" s="22" t="e" vm="34">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="22" t="s">
-        <v>276</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="30">
-        <v>45595</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="F15" s="30">
-        <v>44437</v>
-      </c>
-      <c r="G15" s="30">
-        <v>46630</v>
-      </c>
-      <c r="H15" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I15" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="J15" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="K15" s="22" t="s">
-        <v>238</v>
-      </c>
-      <c r="L15" s="22">
-        <v>5550360000</v>
-      </c>
-      <c r="M15" s="22">
-        <v>62067</v>
-      </c>
-      <c r="N15" s="26" t="s">
-        <v>239</v>
-      </c>
-      <c r="O15" s="26" t="s">
-        <v>240</v>
-      </c>
-      <c r="P15" s="22" t="e" vm="35">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="22" t="s">
-        <v>277</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>242</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="30">
-        <v>44437</v>
-      </c>
-      <c r="G16" s="30">
-        <v>46630</v>
-      </c>
-      <c r="H16" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I16" s="22" t="s">
-        <v>243</v>
-      </c>
-      <c r="J16" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="K16" s="26" t="s">
-        <v>244</v>
-      </c>
-      <c r="L16" s="22">
-        <v>5550360000</v>
-      </c>
-      <c r="M16" s="22">
-        <v>62054</v>
-      </c>
-      <c r="N16" s="26" t="s">
-        <v>245</v>
-      </c>
-      <c r="O16" s="26" t="s">
-        <v>246</v>
-      </c>
-      <c r="P16" s="22" t="e" vm="36">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="22" t="s">
-        <v>278</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>218</v>
-      </c>
-      <c r="C17" s="30">
-        <v>45595</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="F17" s="30">
-        <v>44437</v>
-      </c>
-      <c r="G17" s="30">
-        <v>46630</v>
-      </c>
-      <c r="H17" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="I17" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="J17" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="K17" s="26" t="s">
-        <v>248</v>
-      </c>
-      <c r="L17" s="22">
-        <v>5550360000</v>
-      </c>
-      <c r="M17" s="22">
-        <v>62636</v>
-      </c>
-      <c r="N17" s="26" t="s">
-        <v>249</v>
-      </c>
-      <c r="O17" s="26" t="s">
-        <v>250</v>
-      </c>
-      <c r="P17" s="22" t="e" vm="37">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="22" t="s">
-        <v>279</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="30">
-        <v>45595</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="F18" s="30">
-        <v>44437</v>
-      </c>
-      <c r="G18" s="30">
-        <v>46630</v>
-      </c>
-      <c r="H18" s="22" t="s">
-        <v>252</v>
-      </c>
-      <c r="I18" s="22" t="s">
-        <v>253</v>
-      </c>
-      <c r="J18" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="K18" s="26" t="s">
-        <v>254</v>
-      </c>
-      <c r="L18" s="22">
-        <v>5550360000</v>
-      </c>
-      <c r="M18" s="22">
-        <v>59410</v>
-      </c>
-      <c r="N18" s="26" t="s">
-        <v>255</v>
-      </c>
-      <c r="O18" s="26" t="s">
-        <v>256</v>
-      </c>
-      <c r="P18" s="22" t="e" vm="38">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="22" t="s">
-        <v>280</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="30">
-        <v>45595</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="F19" s="30">
-        <v>44437</v>
-      </c>
-      <c r="G19" s="30">
-        <v>46630</v>
-      </c>
-      <c r="H19" s="22" t="s">
-        <v>252</v>
-      </c>
-      <c r="I19" s="22" t="s">
-        <v>258</v>
-      </c>
-      <c r="J19" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="K19" s="22" t="s">
-        <v>259</v>
-      </c>
-      <c r="L19" s="22">
-        <v>5550360000</v>
-      </c>
-      <c r="M19" s="22">
-        <v>68850</v>
-      </c>
-      <c r="N19" s="26" t="s">
-        <v>260</v>
-      </c>
-      <c r="O19" s="26" t="s">
-        <v>261</v>
-      </c>
-      <c r="P19" s="22" t="e" vm="39">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>262</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1" xr:uid="{F494D8B1-27C6-49D3-8FDD-9A4396888437}"/>
-    <hyperlink ref="O2" r:id="rId2" display="https://sil.gobernacion.gob.mx/Librerias/pp_PerfilLegislador.php?Referencia=9227697" xr:uid="{5B19A580-883E-4B41-9303-21D9AB3641A7}"/>
-    <hyperlink ref="N3" r:id="rId3" xr:uid="{F1388137-65F9-4252-86D9-E7597A1DD03E}"/>
-    <hyperlink ref="O3" r:id="rId4" xr:uid="{5FEE3462-39AB-4EAF-8369-BE80C65E4B90}"/>
-    <hyperlink ref="N4" r:id="rId5" xr:uid="{BBC9461B-0678-411D-B47B-4D1E0EDA5BEF}"/>
-    <hyperlink ref="O4" r:id="rId6" xr:uid="{1815E2D8-2F71-4519-BE39-579D298E3A16}"/>
-    <hyperlink ref="K5" r:id="rId7" xr:uid="{E703AEC8-8E73-4F2A-A17B-1DF7A9E31FDC}"/>
-    <hyperlink ref="N5" r:id="rId8" xr:uid="{0E9EF265-D266-4B65-BF58-2CCD8CC9AACB}"/>
-    <hyperlink ref="O5" r:id="rId9" xr:uid="{5DB6F1C2-79A4-4181-A13A-110DFFAA4D9A}"/>
-    <hyperlink ref="N6" r:id="rId10" xr:uid="{41E8213E-4E3A-4D42-A6BD-0366D39EF74D}"/>
-    <hyperlink ref="O6" r:id="rId11" xr:uid="{82B296D6-8208-4E63-8C9E-1F73B030A4C1}"/>
-    <hyperlink ref="K6" r:id="rId12" xr:uid="{5E2229D4-4652-4AA0-A2B1-388066D5E992}"/>
-    <hyperlink ref="K7" r:id="rId13" xr:uid="{8C40449E-2EBF-4901-B172-1161B5845D72}"/>
-    <hyperlink ref="N7" r:id="rId14" xr:uid="{DF390B30-8E75-496E-B3C6-92B6CABB737B}"/>
-    <hyperlink ref="O7" r:id="rId15" xr:uid="{E32EBEB0-8F27-4EA2-9850-29C1DE3145B2}"/>
-    <hyperlink ref="K8" r:id="rId16" xr:uid="{165CFDFC-5DE9-4941-9AFA-7C473A4B4454}"/>
-    <hyperlink ref="N8" r:id="rId17" xr:uid="{00AF7454-AFD7-4366-AC95-35870231087F}"/>
-    <hyperlink ref="O8" r:id="rId18" xr:uid="{80BD1492-DB63-4558-83F3-1C4EF72F8FC9}"/>
-    <hyperlink ref="K9" r:id="rId19" xr:uid="{A1A3E78F-48C4-4EED-8843-00F80EFD0937}"/>
-    <hyperlink ref="N9" r:id="rId20" xr:uid="{AE92BE08-5DCE-43F1-9BDF-790B2864E8DD}"/>
-    <hyperlink ref="O9" r:id="rId21" xr:uid="{D185C4FB-45FE-44B7-B513-16E611CC42C2}"/>
-    <hyperlink ref="K10" r:id="rId22" xr:uid="{C3D291B8-CD03-404D-B656-FFE8C257F9C0}"/>
-    <hyperlink ref="N10" r:id="rId23" xr:uid="{82AC9C62-8987-4D28-971D-FBDAEBC5A597}"/>
-    <hyperlink ref="O10" r:id="rId24" xr:uid="{ABCC48D5-E5D2-4BC0-B0A5-04198F7F8AD0}"/>
-    <hyperlink ref="N11" r:id="rId25" xr:uid="{69B211E6-239D-48D7-8D88-F7E2991CBE8C}"/>
-    <hyperlink ref="O11" r:id="rId26" xr:uid="{6555C734-4D37-49E4-A153-0C776E9B84B4}"/>
-    <hyperlink ref="N12" r:id="rId27" xr:uid="{106AE3DA-6EBF-43CF-BAE0-CD36A4658FDE}"/>
-    <hyperlink ref="O12" r:id="rId28" xr:uid="{DF775BD4-8237-47A7-9094-7AAC4D78AFF4}"/>
-    <hyperlink ref="N13" r:id="rId29" xr:uid="{ABB1B2ED-0A30-488B-8515-B66E02F1D1A4}"/>
-    <hyperlink ref="O13" r:id="rId30" xr:uid="{869870C5-5119-415F-9A07-CD39FAB22D56}"/>
-    <hyperlink ref="N14" r:id="rId31" xr:uid="{0E9AB998-45B2-4109-B4CF-D8BEB382A174}"/>
-    <hyperlink ref="O14" r:id="rId32" xr:uid="{4DC7DD20-9026-4B66-988E-23B823CB28EC}"/>
-    <hyperlink ref="N15" r:id="rId33" xr:uid="{994283AA-16AC-44C8-8780-AA7B390BF5C3}"/>
-    <hyperlink ref="O15" r:id="rId34" location="PerfiLegislador" xr:uid="{F7E818F6-85ED-41B4-A012-E2424A6F1FB9}"/>
-    <hyperlink ref="K16" r:id="rId35" xr:uid="{0D7A8C28-767C-48E9-B602-16C2E50CAC9B}"/>
-    <hyperlink ref="N16" r:id="rId36" xr:uid="{48A3ED08-0ECD-4DFD-8889-844FF9DA52B5}"/>
-    <hyperlink ref="O16" r:id="rId37" xr:uid="{7D368797-4789-4A79-92D6-201E097EC361}"/>
-    <hyperlink ref="K17" r:id="rId38" xr:uid="{D0F9196F-0A9D-4F69-8509-F1FEEB09E565}"/>
-    <hyperlink ref="N17" r:id="rId39" xr:uid="{0283BAB0-C844-44C5-B2F2-2E7127C0DCBF}"/>
-    <hyperlink ref="O17" r:id="rId40" xr:uid="{9B71341F-F7C9-4D0E-BC8E-E7E8F0CA1C75}"/>
-    <hyperlink ref="K18" r:id="rId41" xr:uid="{225E9022-C9CC-48E9-84D5-4AA8EADDE397}"/>
-    <hyperlink ref="N18" r:id="rId42" xr:uid="{1CFA5889-0439-4365-B00C-BB5521AF2CC0}"/>
-    <hyperlink ref="O18" r:id="rId43" xr:uid="{9CE466C4-AF07-4271-B133-56EA385BFC65}"/>
-    <hyperlink ref="N19" r:id="rId44" xr:uid="{1378D7C7-AAC3-4E37-A62B-F73A5997F15E}"/>
-    <hyperlink ref="O19" r:id="rId45" xr:uid="{F5C742A3-121F-48DE-87FF-BECBA6D75D75}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5271,18 +5356,18 @@
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.36328125" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" customWidth="1"/>
-    <col min="5" max="5" width="24.90625" customWidth="1"/>
-    <col min="6" max="6" width="11.08984375" customWidth="1"/>
-    <col min="7" max="7" width="10.90625" customWidth="1"/>
+    <col min="1" max="1" width="45.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>139</v>
       </c>
@@ -5303,7 +5388,7 @@
       </c>
       <c r="G1" s="14"/>
     </row>
-    <row r="2" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>263</v>
       </c>
@@ -5327,7 +5412,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>264</v>
       </c>
@@ -5351,7 +5436,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>265</v>
       </c>
@@ -5375,7 +5460,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>266</v>
       </c>
@@ -5399,7 +5484,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>267</v>
       </c>
@@ -5423,7 +5508,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>268</v>
       </c>
@@ -5447,7 +5532,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>269</v>
       </c>
@@ -5471,7 +5556,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>270</v>
       </c>
@@ -5495,7 +5580,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>271</v>
       </c>
@@ -5519,7 +5604,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>272</v>
       </c>
@@ -5543,7 +5628,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>273</v>
       </c>
@@ -5567,7 +5652,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>274</v>
       </c>
@@ -5591,7 +5676,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>275</v>
       </c>
@@ -5615,7 +5700,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>276</v>
       </c>
@@ -5639,7 +5724,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>277</v>
       </c>
@@ -5663,7 +5748,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>278</v>
       </c>
@@ -5687,7 +5772,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>279</v>
       </c>
@@ -5711,7 +5796,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>280</v>
       </c>

</xml_diff>